<commit_message>
excel add chart test
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -71,16 +71,22 @@
     <t>3256</t>
   </si>
   <si>
+    <t>SearchIndexer.exe</t>
+  </si>
+  <si>
+    <t>3764</t>
+  </si>
+  <si>
     <t>ExpressTray.exe</t>
   </si>
   <si>
     <t>4220</t>
   </si>
   <si>
-    <t>SearchIndexer.exe</t>
-  </si>
-  <si>
-    <t>3764</t>
+    <t>dwm.exe</t>
+  </si>
+  <si>
+    <t>884</t>
   </si>
   <si>
     <t>Garmin.Cartography.MapUpdate.CoreService.exe</t>
@@ -101,16 +107,16 @@
     <t>3296</t>
   </si>
   <si>
-    <t>dwm.exe</t>
-  </si>
-  <si>
-    <t>884</t>
-  </si>
-  <si>
     <t>java.exe</t>
   </si>
   <si>
-    <t>6912</t>
+    <t>7680</t>
+  </si>
+  <si>
+    <t>IAStorIcon.exe</t>
+  </si>
+  <si>
+    <t>4072</t>
   </si>
   <si>
     <t>taskhostex.exe</t>
@@ -119,112 +125,112 @@
     <t>3304</t>
   </si>
   <si>
-    <t>IAStorIcon.exe</t>
-  </si>
-  <si>
-    <t>4072</t>
-  </si>
-  <si>
     <t>OSPPSVC.EXE</t>
   </si>
   <si>
     <t>8100</t>
   </si>
   <si>
+    <t>RuntimeBroker.exe</t>
+  </si>
+  <si>
+    <t>2196</t>
+  </si>
+  <si>
     <t>csrss.exe</t>
   </si>
   <si>
     <t>496</t>
   </si>
   <si>
-    <t>RuntimeBroker.exe</t>
-  </si>
-  <si>
-    <t>2196</t>
+    <t>lsass.exe</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>spd.exe</t>
+  </si>
+  <si>
+    <t>1588</t>
+  </si>
+  <si>
+    <t>cfosspeed.exe</t>
+  </si>
+  <si>
+    <t>584</t>
+  </si>
+  <si>
+    <t>dasHost.exe</t>
+  </si>
+  <si>
+    <t>2968</t>
+  </si>
+  <si>
+    <t>WmiPrvSE.exe</t>
+  </si>
+  <si>
+    <t>4088</t>
+  </si>
+  <si>
+    <t>MpCmdRun.exe</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>4game-service.exe</t>
+  </si>
+  <si>
+    <t>1484</t>
   </si>
   <si>
     <t>SearchFilterHost.exe</t>
   </si>
   <si>
-    <t>7552</t>
-  </si>
-  <si>
-    <t>lsass.exe</t>
-  </si>
-  <si>
-    <t>684</t>
-  </si>
-  <si>
-    <t>audiodg.exe</t>
-  </si>
-  <si>
-    <t>7900</t>
-  </si>
-  <si>
-    <t>spd.exe</t>
-  </si>
-  <si>
-    <t>1588</t>
-  </si>
-  <si>
-    <t>cfosspeed.exe</t>
-  </si>
-  <si>
-    <t>584</t>
-  </si>
-  <si>
-    <t>dasHost.exe</t>
-  </si>
-  <si>
-    <t>2968</t>
-  </si>
-  <si>
-    <t>WmiPrvSE.exe</t>
-  </si>
-  <si>
-    <t>4088</t>
-  </si>
-  <si>
-    <t>MpCmdRun.exe</t>
-  </si>
-  <si>
-    <t>4800</t>
-  </si>
-  <si>
-    <t>4game-service.exe</t>
-  </si>
-  <si>
-    <t>1484</t>
+    <t>2332</t>
+  </si>
+  <si>
+    <t>iSCTAgent.exe</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>CCC.exe</t>
+  </si>
+  <si>
+    <t>4684</t>
+  </si>
+  <si>
+    <t>conhost.exe</t>
+  </si>
+  <si>
+    <t>6552</t>
+  </si>
+  <si>
+    <t>RAVCpl64.exe</t>
+  </si>
+  <si>
+    <t>4112</t>
+  </si>
+  <si>
+    <t>jusched.exe</t>
+  </si>
+  <si>
+    <t>4328</t>
+  </si>
+  <si>
+    <t>MOM.exe</t>
+  </si>
+  <si>
+    <t>4320</t>
   </si>
   <si>
     <t>SearchProtocolHost.exe</t>
   </si>
   <si>
-    <t>2460</t>
-  </si>
-  <si>
-    <t>iSCTAgent.exe</t>
-  </si>
-  <si>
-    <t>1220</t>
-  </si>
-  <si>
-    <t>conhost.exe</t>
-  </si>
-  <si>
-    <t>6180</t>
-  </si>
-  <si>
-    <t>RAVCpl64.exe</t>
-  </si>
-  <si>
-    <t>4112</t>
-  </si>
-  <si>
-    <t>jusched.exe</t>
-  </si>
-  <si>
-    <t>4328</t>
+    <t>4668</t>
   </si>
   <si>
     <t>spoolsv.exe</t>
@@ -242,7 +248,7 @@
     <t>tasklist.exe</t>
   </si>
   <si>
-    <t>5072</t>
+    <t>3232</t>
   </si>
   <si>
     <t>mdm.exe</t>
@@ -263,34 +269,22 @@
     <t>2808</t>
   </si>
   <si>
-    <t>CCC.exe</t>
-  </si>
-  <si>
-    <t>4684</t>
-  </si>
-  <si>
     <t>winlogon.exe</t>
   </si>
   <si>
     <t>648</t>
   </si>
   <si>
-    <t>taskeng.exe</t>
-  </si>
-  <si>
-    <t>4752</t>
-  </si>
-  <si>
     <t>slimsvc.exe</t>
   </si>
   <si>
     <t>1616</t>
   </si>
   <si>
-    <t>MOM.exe</t>
-  </si>
-  <si>
-    <t>4320</t>
+    <t>NisSrv.exe</t>
+  </si>
+  <si>
+    <t>4400</t>
   </si>
   <si>
     <t>sqlwriter.exe</t>
@@ -381,12 +375,6 @@
   </si>
   <si>
     <t>1124</t>
-  </si>
-  <si>
-    <t>NisSrv.exe</t>
-  </si>
-  <si>
-    <t>4400</t>
   </si>
   <si>
     <t>System Idle Process</t>
@@ -435,8 +423,298 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="false"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$61</c:f>
+              <c:numCache>
+                <c:ptCount val="60"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$61</c:f>
+              <c:numCache>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>5701920.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1198328.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>274460.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128352.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120376.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107116.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102336.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78804.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35888.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32892.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29368.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27712.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26256.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24420.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20108.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16828.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16780.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11924.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11496.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11384.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10940.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10316.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9180.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9092.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8648.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8476.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8232.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8136.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7764.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7640.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6940.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6936.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6856.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6512.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6072.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5876.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5836.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5740.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5712.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5584.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4996.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4604.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4568.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4184.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4164.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4112.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4008.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3580.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3428.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3380.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3304.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3124.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3116.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2940.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1792.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>848.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>572.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>528.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="false"/>
+    </c:legend>
+    <c:plotVisOnly val="true"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
@@ -462,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4064984.0</v>
+        <v>5701920.0</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1139268.0</v>
+        <v>1198328.0</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>257484.0</v>
+        <v>274460.0</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>131716.0</v>
+        <v>128352.0</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +784,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>119476.0</v>
+        <v>120376.0</v>
       </c>
     </row>
     <row r="7">
@@ -517,7 +795,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>103708.0</v>
+        <v>107116.0</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +806,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>97984.0</v>
+        <v>102336.0</v>
       </c>
     </row>
     <row r="9">
@@ -539,7 +817,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>78832.0</v>
+        <v>78804.0</v>
       </c>
     </row>
     <row r="10">
@@ -550,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>32800.0</v>
+        <v>35888.0</v>
       </c>
     </row>
     <row r="11">
@@ -561,7 +839,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>31912.0</v>
+        <v>32892.0</v>
       </c>
     </row>
     <row r="12">
@@ -572,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="n">
-        <v>27096.0</v>
+        <v>29368.0</v>
       </c>
     </row>
     <row r="13">
@@ -583,7 +861,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="n">
-        <v>25216.0</v>
+        <v>27712.0</v>
       </c>
     </row>
     <row r="14">
@@ -594,7 +872,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="n">
-        <v>22664.0</v>
+        <v>26256.0</v>
       </c>
     </row>
     <row r="15">
@@ -605,7 +883,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>21296.0</v>
+        <v>24420.0</v>
       </c>
     </row>
     <row r="16">
@@ -616,7 +894,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="n">
-        <v>20252.0</v>
+        <v>20108.0</v>
       </c>
     </row>
     <row r="17">
@@ -627,7 +905,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="n">
-        <v>16916.0</v>
+        <v>16828.0</v>
       </c>
     </row>
     <row r="18">
@@ -638,7 +916,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="n">
-        <v>16828.0</v>
+        <v>16780.0</v>
       </c>
     </row>
     <row r="19">
@@ -649,7 +927,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="n">
-        <v>11820.0</v>
+        <v>11924.0</v>
       </c>
     </row>
     <row r="20">
@@ -660,7 +938,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="n">
-        <v>11676.0</v>
+        <v>11496.0</v>
       </c>
     </row>
     <row r="21">
@@ -671,7 +949,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="n">
-        <v>11496.0</v>
+        <v>11384.0</v>
       </c>
     </row>
     <row r="22">
@@ -682,7 +960,7 @@
         <v>44</v>
       </c>
       <c r="C22" t="n">
-        <v>11196.0</v>
+        <v>10940.0</v>
       </c>
     </row>
     <row r="23">
@@ -693,7 +971,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="n">
-        <v>10776.0</v>
+        <v>10316.0</v>
       </c>
     </row>
     <row r="24">
@@ -704,7 +982,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="n">
-        <v>10712.0</v>
+        <v>9180.0</v>
       </c>
     </row>
     <row r="25">
@@ -715,7 +993,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>10236.0</v>
+        <v>9092.0</v>
       </c>
     </row>
     <row r="26">
@@ -726,7 +1004,7 @@
         <v>52</v>
       </c>
       <c r="C26" t="n">
-        <v>9176.0</v>
+        <v>8648.0</v>
       </c>
     </row>
     <row r="27">
@@ -737,7 +1015,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="n">
-        <v>9092.0</v>
+        <v>8476.0</v>
       </c>
     </row>
     <row r="28">
@@ -748,7 +1026,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="n">
-        <v>8800.0</v>
+        <v>8232.0</v>
       </c>
     </row>
     <row r="29">
@@ -759,7 +1037,7 @@
         <v>58</v>
       </c>
       <c r="C29" t="n">
-        <v>8516.0</v>
+        <v>8136.0</v>
       </c>
     </row>
     <row r="30">
@@ -770,7 +1048,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="n">
-        <v>8376.0</v>
+        <v>7764.0</v>
       </c>
     </row>
     <row r="31">
@@ -781,7 +1059,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="n">
-        <v>8268.0</v>
+        <v>7640.0</v>
       </c>
     </row>
     <row r="32">
@@ -792,7 +1070,7 @@
         <v>64</v>
       </c>
       <c r="C32" t="n">
-        <v>7764.0</v>
+        <v>6940.0</v>
       </c>
     </row>
     <row r="33">
@@ -803,7 +1081,7 @@
         <v>66</v>
       </c>
       <c r="C33" t="n">
-        <v>6968.0</v>
+        <v>6936.0</v>
       </c>
     </row>
     <row r="34">
@@ -814,7 +1092,7 @@
         <v>68</v>
       </c>
       <c r="C34" t="n">
-        <v>6936.0</v>
+        <v>6856.0</v>
       </c>
     </row>
     <row r="35">
@@ -825,7 +1103,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="n">
-        <v>6856.0</v>
+        <v>6512.0</v>
       </c>
     </row>
     <row r="36">
@@ -836,7 +1114,7 @@
         <v>72</v>
       </c>
       <c r="C36" t="n">
-        <v>6072.0</v>
+        <v>6500.0</v>
       </c>
     </row>
     <row r="37">
@@ -847,7 +1125,7 @@
         <v>74</v>
       </c>
       <c r="C37" t="n">
-        <v>5876.0</v>
+        <v>6072.0</v>
       </c>
     </row>
     <row r="38">
@@ -858,7 +1136,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="n">
-        <v>5804.0</v>
+        <v>5876.0</v>
       </c>
     </row>
     <row r="39">
@@ -869,7 +1147,7 @@
         <v>78</v>
       </c>
       <c r="C39" t="n">
-        <v>5740.0</v>
+        <v>5836.0</v>
       </c>
     </row>
     <row r="40">
@@ -880,7 +1158,7 @@
         <v>80</v>
       </c>
       <c r="C40" t="n">
-        <v>5708.0</v>
+        <v>5740.0</v>
       </c>
     </row>
     <row r="41">
@@ -891,7 +1169,7 @@
         <v>82</v>
       </c>
       <c r="C41" t="n">
-        <v>5584.0</v>
+        <v>5712.0</v>
       </c>
     </row>
     <row r="42">
@@ -902,7 +1180,7 @@
         <v>84</v>
       </c>
       <c r="C42" t="n">
-        <v>5188.0</v>
+        <v>5584.0</v>
       </c>
     </row>
     <row r="43">
@@ -924,7 +1202,7 @@
         <v>88</v>
       </c>
       <c r="C44" t="n">
-        <v>4784.0</v>
+        <v>4604.0</v>
       </c>
     </row>
     <row r="45">
@@ -935,7 +1213,7 @@
         <v>90</v>
       </c>
       <c r="C45" t="n">
-        <v>4604.0</v>
+        <v>4568.0</v>
       </c>
     </row>
     <row r="46">
@@ -946,7 +1224,7 @@
         <v>92</v>
       </c>
       <c r="C46" t="n">
-        <v>4580.0</v>
+        <v>4184.0</v>
       </c>
     </row>
     <row r="47">
@@ -957,7 +1235,7 @@
         <v>94</v>
       </c>
       <c r="C47" t="n">
-        <v>4184.0</v>
+        <v>4164.0</v>
       </c>
     </row>
     <row r="48">
@@ -968,7 +1246,7 @@
         <v>96</v>
       </c>
       <c r="C48" t="n">
-        <v>4164.0</v>
+        <v>4112.0</v>
       </c>
     </row>
     <row r="49">
@@ -979,7 +1257,7 @@
         <v>98</v>
       </c>
       <c r="C49" t="n">
-        <v>4112.0</v>
+        <v>4008.0</v>
       </c>
     </row>
     <row r="50">
@@ -990,7 +1268,7 @@
         <v>100</v>
       </c>
       <c r="C50" t="n">
-        <v>4008.0</v>
+        <v>3580.0</v>
       </c>
     </row>
     <row r="51">
@@ -1001,7 +1279,7 @@
         <v>102</v>
       </c>
       <c r="C51" t="n">
-        <v>3580.0</v>
+        <v>3428.0</v>
       </c>
     </row>
     <row r="52">
@@ -1012,7 +1290,7 @@
         <v>104</v>
       </c>
       <c r="C52" t="n">
-        <v>3428.0</v>
+        <v>3380.0</v>
       </c>
     </row>
     <row r="53">
@@ -1023,7 +1301,7 @@
         <v>106</v>
       </c>
       <c r="C53" t="n">
-        <v>3380.0</v>
+        <v>3304.0</v>
       </c>
     </row>
     <row r="54">
@@ -1034,7 +1312,7 @@
         <v>108</v>
       </c>
       <c r="C54" t="n">
-        <v>3304.0</v>
+        <v>3124.0</v>
       </c>
     </row>
     <row r="55">
@@ -1045,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="C55" t="n">
-        <v>3124.0</v>
+        <v>3116.0</v>
       </c>
     </row>
     <row r="56">
@@ -1056,7 +1334,7 @@
         <v>112</v>
       </c>
       <c r="C56" t="n">
-        <v>3116.0</v>
+        <v>2940.0</v>
       </c>
     </row>
     <row r="57">
@@ -1067,7 +1345,7 @@
         <v>114</v>
       </c>
       <c r="C57" t="n">
-        <v>2940.0</v>
+        <v>1792.0</v>
       </c>
     </row>
     <row r="58">
@@ -1078,7 +1356,7 @@
         <v>116</v>
       </c>
       <c r="C58" t="n">
-        <v>1760.0</v>
+        <v>848.0</v>
       </c>
     </row>
     <row r="59">
@@ -1089,7 +1367,7 @@
         <v>118</v>
       </c>
       <c r="C59" t="n">
-        <v>848.0</v>
+        <v>572.0</v>
       </c>
     </row>
     <row r="60">
@@ -1100,7 +1378,7 @@
         <v>120</v>
       </c>
       <c r="C60" t="n">
-        <v>572.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="61">
@@ -1111,32 +1389,11 @@
         <v>122</v>
       </c>
       <c r="C61" t="n">
-        <v>528.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" t="n">
-        <v>192.0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" t="n">
         <v>4.0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>